<commit_message>
update spike soritng notes and rfmap info
</commit_message>
<xml_diff>
--- a/spikeSortingNotes.xlsx
+++ b/spikeSortingNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\MATLAB\gratings-task-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A29B27B-9152-48CA-8981-5B4BB167CC73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210F25DF-C7F9-4DDD-9F3B-C32B49F61E20}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="495" windowWidth="18015" windowHeight="14955" xr2:uid="{F5215BA6-879C-42E2-A238-7256D4555DD7}"/>
+    <workbookView xWindow="135" yWindow="330" windowWidth="18015" windowHeight="14955" xr2:uid="{F5215BA6-879C-42E2-A238-7256D4555DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Unit Info" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5230" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5554" uniqueCount="483">
   <si>
     <t>Session</t>
   </si>
@@ -1431,6 +1431,57 @@
   <si>
     <t>Super sparse</t>
   </si>
+  <si>
+    <t>F20171101</t>
+  </si>
+  <si>
+    <t>May be axon because of early positivity</t>
+  </si>
+  <si>
+    <t>May be axon. Trough to peak duration 175 ms</t>
+  </si>
+  <si>
+    <t>Sharp triphasic, trough to peak duration 100 ms</t>
+  </si>
+  <si>
+    <t>Broad trough or double trough, combined early and late</t>
+  </si>
+  <si>
+    <t>Could be axon, trough to peak duration 175 ms, kinda sharp</t>
+  </si>
+  <si>
+    <t>Sharp triphasic trough to peak duration 150 ms</t>
+  </si>
+  <si>
+    <t>Broad triphasic</t>
+  </si>
+  <si>
+    <t>Kinda triphasic but trough to peak duration is 200 ms and first peak is low</t>
+  </si>
+  <si>
+    <t>Trough to peak duration 160 ms, low amplitude</t>
+  </si>
+  <si>
+    <t>F20171106</t>
+  </si>
+  <si>
+    <t>Double trough, early, left separate from b</t>
+  </si>
+  <si>
+    <t>Double trough, late</t>
+  </si>
+  <si>
+    <t>Short trough to peak duration and slightly triphasic. More likely NS but possibly axon</t>
+  </si>
+  <si>
+    <t>Slightly triphasic but long trough to peak time so more likely NS</t>
+  </si>
+  <si>
+    <t>No clear unit except in first 900 s</t>
+  </si>
+  <si>
+    <t>Biphasic, but too sharp, trough to peak duration 150 ms</t>
+  </si>
 </sst>
 </file>
 
@@ -1793,10 +1844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991F1F63-41CC-4425-B140-2A823B1406A8}">
-  <dimension ref="A1:H3856"/>
+  <dimension ref="A1:H4069"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3393" workbookViewId="0">
-      <selection activeCell="E3421" sqref="E3421"/>
+    <sheetView tabSelected="1" topLeftCell="A3936" workbookViewId="0">
+      <selection activeCell="A3956" sqref="A3956:A4069"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -74120,6 +74171,4275 @@
       </c>
       <c r="H3856" t="s">
         <v>456</v>
+      </c>
+    </row>
+    <row r="3857" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3857" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3857">
+        <v>1</v>
+      </c>
+      <c r="C3857">
+        <v>0</v>
+      </c>
+      <c r="D3857">
+        <v>0</v>
+      </c>
+      <c r="E3857">
+        <v>0</v>
+      </c>
+      <c r="H3857" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3858" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3858" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3858">
+        <v>2</v>
+      </c>
+      <c r="C3858">
+        <v>0</v>
+      </c>
+      <c r="D3858">
+        <v>0</v>
+      </c>
+      <c r="E3858">
+        <v>0</v>
+      </c>
+      <c r="H3858" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3859" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3859" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3859">
+        <v>3</v>
+      </c>
+      <c r="C3859">
+        <v>0</v>
+      </c>
+      <c r="D3859">
+        <v>0</v>
+      </c>
+      <c r="E3859">
+        <v>0</v>
+      </c>
+      <c r="H3859" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3860" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3860" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3860">
+        <v>4</v>
+      </c>
+      <c r="C3860">
+        <v>0</v>
+      </c>
+      <c r="D3860">
+        <v>0</v>
+      </c>
+      <c r="E3860">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3861" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3861" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3861">
+        <v>4</v>
+      </c>
+      <c r="C3861">
+        <v>1</v>
+      </c>
+      <c r="D3861">
+        <v>1</v>
+      </c>
+      <c r="E3861">
+        <v>3</v>
+      </c>
+      <c r="G3861">
+        <v>1800</v>
+      </c>
+      <c r="H3861" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="3862" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3862" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3862">
+        <v>5</v>
+      </c>
+      <c r="C3862">
+        <v>0</v>
+      </c>
+      <c r="D3862">
+        <v>0</v>
+      </c>
+      <c r="E3862">
+        <v>0</v>
+      </c>
+      <c r="H3862" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3863" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3863" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3863">
+        <v>6</v>
+      </c>
+      <c r="C3863">
+        <v>0</v>
+      </c>
+      <c r="D3863">
+        <v>0</v>
+      </c>
+      <c r="E3863">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3864" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3864" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3864">
+        <v>6</v>
+      </c>
+      <c r="C3864">
+        <v>1</v>
+      </c>
+      <c r="D3864">
+        <v>1</v>
+      </c>
+      <c r="E3864">
+        <v>4</v>
+      </c>
+      <c r="F3864">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="3865" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3865" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3865">
+        <v>6</v>
+      </c>
+      <c r="C3865">
+        <v>2</v>
+      </c>
+      <c r="D3865">
+        <v>1</v>
+      </c>
+      <c r="E3865">
+        <v>5</v>
+      </c>
+      <c r="F3865">
+        <v>900</v>
+      </c>
+      <c r="G3865">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="3866" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3866" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3866">
+        <v>6</v>
+      </c>
+      <c r="C3866">
+        <v>3</v>
+      </c>
+      <c r="D3866">
+        <v>1</v>
+      </c>
+      <c r="E3866">
+        <v>3</v>
+      </c>
+      <c r="F3866">
+        <v>6300</v>
+      </c>
+      <c r="H3866" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3867" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3867" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3867">
+        <v>7</v>
+      </c>
+      <c r="C3867">
+        <v>0</v>
+      </c>
+      <c r="D3867">
+        <v>0</v>
+      </c>
+      <c r="E3867">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3868" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3868" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3868">
+        <v>7</v>
+      </c>
+      <c r="C3868">
+        <v>1</v>
+      </c>
+      <c r="D3868">
+        <v>1</v>
+      </c>
+      <c r="E3868">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3869" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3869" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3869">
+        <v>8</v>
+      </c>
+      <c r="C3869">
+        <v>0</v>
+      </c>
+      <c r="D3869">
+        <v>0</v>
+      </c>
+      <c r="E3869">
+        <v>0</v>
+      </c>
+      <c r="H3869" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3870" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3870" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3870">
+        <v>9</v>
+      </c>
+      <c r="C3870">
+        <v>0</v>
+      </c>
+      <c r="D3870">
+        <v>0</v>
+      </c>
+      <c r="E3870">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3871" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3871" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3871">
+        <v>9</v>
+      </c>
+      <c r="C3871">
+        <v>1</v>
+      </c>
+      <c r="D3871">
+        <v>1</v>
+      </c>
+      <c r="E3871">
+        <v>4</v>
+      </c>
+      <c r="F3871">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="3872" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3872" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3872">
+        <v>10</v>
+      </c>
+      <c r="C3872">
+        <v>0</v>
+      </c>
+      <c r="D3872">
+        <v>0</v>
+      </c>
+      <c r="E3872">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3873" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3873" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3873">
+        <v>10</v>
+      </c>
+      <c r="C3873">
+        <v>1</v>
+      </c>
+      <c r="D3873">
+        <v>1</v>
+      </c>
+      <c r="E3873">
+        <v>2</v>
+      </c>
+      <c r="F3873">
+        <v>9000</v>
+      </c>
+      <c r="H3873" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3874" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3874" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3874">
+        <v>11</v>
+      </c>
+      <c r="C3874">
+        <v>0</v>
+      </c>
+      <c r="D3874">
+        <v>0</v>
+      </c>
+      <c r="E3874">
+        <v>0</v>
+      </c>
+      <c r="H3874" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3875" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3875" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3875">
+        <v>12</v>
+      </c>
+      <c r="C3875">
+        <v>0</v>
+      </c>
+      <c r="D3875">
+        <v>0</v>
+      </c>
+      <c r="E3875">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3876" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3876" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3876">
+        <v>12</v>
+      </c>
+      <c r="C3876">
+        <v>1</v>
+      </c>
+      <c r="D3876">
+        <v>1</v>
+      </c>
+      <c r="E3876">
+        <v>3</v>
+      </c>
+      <c r="F3876">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="3877" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3877" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3877">
+        <v>13</v>
+      </c>
+      <c r="C3877">
+        <v>0</v>
+      </c>
+      <c r="D3877">
+        <v>0</v>
+      </c>
+      <c r="E3877">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3878" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3878" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3878">
+        <v>13</v>
+      </c>
+      <c r="C3878">
+        <v>1</v>
+      </c>
+      <c r="D3878">
+        <v>1</v>
+      </c>
+      <c r="E3878">
+        <v>2</v>
+      </c>
+      <c r="F3878">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="3879" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3879" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3879">
+        <v>14</v>
+      </c>
+      <c r="C3879">
+        <v>0</v>
+      </c>
+      <c r="D3879">
+        <v>0</v>
+      </c>
+      <c r="E3879">
+        <v>0</v>
+      </c>
+      <c r="H3879" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3880" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3880" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3880">
+        <v>15</v>
+      </c>
+      <c r="C3880">
+        <v>0</v>
+      </c>
+      <c r="D3880">
+        <v>0</v>
+      </c>
+      <c r="E3880">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3881" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3881" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3881">
+        <v>15</v>
+      </c>
+      <c r="C3881">
+        <v>1</v>
+      </c>
+      <c r="D3881">
+        <v>1</v>
+      </c>
+      <c r="E3881">
+        <v>3</v>
+      </c>
+      <c r="F3881">
+        <v>900</v>
+      </c>
+      <c r="G3881">
+        <v>6300</v>
+      </c>
+    </row>
+    <row r="3882" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3882" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3882">
+        <v>15</v>
+      </c>
+      <c r="C3882">
+        <v>2</v>
+      </c>
+      <c r="D3882">
+        <v>1</v>
+      </c>
+      <c r="E3882">
+        <v>1</v>
+      </c>
+      <c r="F3882">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="3883" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3883" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3883">
+        <v>16</v>
+      </c>
+      <c r="C3883">
+        <v>0</v>
+      </c>
+      <c r="D3883">
+        <v>0</v>
+      </c>
+      <c r="E3883">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3884" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3884" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3884">
+        <v>16</v>
+      </c>
+      <c r="C3884">
+        <v>1</v>
+      </c>
+      <c r="D3884">
+        <v>0</v>
+      </c>
+      <c r="E3884">
+        <v>3</v>
+      </c>
+      <c r="F3884">
+        <v>900</v>
+      </c>
+      <c r="G3884">
+        <v>7200</v>
+      </c>
+      <c r="H3884" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="3885" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3885" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3885">
+        <v>17</v>
+      </c>
+      <c r="C3885">
+        <v>0</v>
+      </c>
+      <c r="D3885">
+        <v>0</v>
+      </c>
+      <c r="E3885">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3886" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3886" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3886">
+        <v>17</v>
+      </c>
+      <c r="C3886">
+        <v>1</v>
+      </c>
+      <c r="D3886">
+        <v>1</v>
+      </c>
+      <c r="E3886">
+        <v>3</v>
+      </c>
+      <c r="F3886">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="3887" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3887" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3887">
+        <v>18</v>
+      </c>
+      <c r="C3887">
+        <v>0</v>
+      </c>
+      <c r="D3887">
+        <v>0</v>
+      </c>
+      <c r="E3887">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3888" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3888" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3888">
+        <v>18</v>
+      </c>
+      <c r="C3888">
+        <v>1</v>
+      </c>
+      <c r="D3888">
+        <v>0</v>
+      </c>
+      <c r="E3888">
+        <v>5</v>
+      </c>
+      <c r="F3888">
+        <v>900</v>
+      </c>
+      <c r="G3888">
+        <v>4500</v>
+      </c>
+      <c r="H3888" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="3889" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3889" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3889">
+        <v>19</v>
+      </c>
+      <c r="C3889">
+        <v>0</v>
+      </c>
+      <c r="D3889">
+        <v>0</v>
+      </c>
+      <c r="E3889">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3890" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3890" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3890">
+        <v>19</v>
+      </c>
+      <c r="C3890">
+        <v>1</v>
+      </c>
+      <c r="D3890">
+        <v>1</v>
+      </c>
+      <c r="E3890">
+        <v>4</v>
+      </c>
+      <c r="F3890">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="3891" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3891" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3891">
+        <v>19</v>
+      </c>
+      <c r="C3891">
+        <v>2</v>
+      </c>
+      <c r="D3891">
+        <v>1</v>
+      </c>
+      <c r="E3891">
+        <v>3</v>
+      </c>
+      <c r="G3891">
+        <v>9000</v>
+      </c>
+      <c r="H3891" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="3892" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3892" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3892">
+        <v>20</v>
+      </c>
+      <c r="C3892">
+        <v>0</v>
+      </c>
+      <c r="D3892">
+        <v>0</v>
+      </c>
+      <c r="E3892">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3893" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3893" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3893">
+        <v>20</v>
+      </c>
+      <c r="C3893">
+        <v>1</v>
+      </c>
+      <c r="D3893">
+        <v>1</v>
+      </c>
+      <c r="E3893">
+        <v>3</v>
+      </c>
+      <c r="F3893">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="3894" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3894" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3894">
+        <v>21</v>
+      </c>
+      <c r="C3894">
+        <v>0</v>
+      </c>
+      <c r="D3894">
+        <v>0</v>
+      </c>
+      <c r="E3894">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3895" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3895" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3895">
+        <v>21</v>
+      </c>
+      <c r="C3895">
+        <v>1</v>
+      </c>
+      <c r="D3895">
+        <v>1</v>
+      </c>
+      <c r="E3895">
+        <v>2</v>
+      </c>
+      <c r="F3895">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="3896" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3896" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3896">
+        <v>22</v>
+      </c>
+      <c r="C3896">
+        <v>0</v>
+      </c>
+      <c r="D3896">
+        <v>0</v>
+      </c>
+      <c r="E3896">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3897" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3897" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3897">
+        <v>22</v>
+      </c>
+      <c r="C3897">
+        <v>1</v>
+      </c>
+      <c r="D3897">
+        <v>1</v>
+      </c>
+      <c r="E3897">
+        <v>3</v>
+      </c>
+      <c r="F3897">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="3898" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3898" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3898">
+        <v>23</v>
+      </c>
+      <c r="C3898">
+        <v>0</v>
+      </c>
+      <c r="D3898">
+        <v>0</v>
+      </c>
+      <c r="E3898">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3899" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3899" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3899">
+        <v>23</v>
+      </c>
+      <c r="C3899">
+        <v>1</v>
+      </c>
+      <c r="D3899">
+        <v>1</v>
+      </c>
+      <c r="E3899">
+        <v>3</v>
+      </c>
+      <c r="F3899">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="3900" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3900" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3900">
+        <v>24</v>
+      </c>
+      <c r="C3900">
+        <v>0</v>
+      </c>
+      <c r="D3900">
+        <v>0</v>
+      </c>
+      <c r="E3900">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3901" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3901" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3901">
+        <v>24</v>
+      </c>
+      <c r="C3901">
+        <v>1</v>
+      </c>
+      <c r="D3901">
+        <v>0</v>
+      </c>
+      <c r="E3901">
+        <v>3</v>
+      </c>
+      <c r="F3901">
+        <v>2700</v>
+      </c>
+      <c r="H3901" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="3902" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3902" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3902">
+        <v>24</v>
+      </c>
+      <c r="C3902">
+        <v>2</v>
+      </c>
+      <c r="D3902">
+        <v>1</v>
+      </c>
+      <c r="E3902">
+        <v>2</v>
+      </c>
+      <c r="F3902">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="3903" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3903" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3903">
+        <v>25</v>
+      </c>
+      <c r="C3903">
+        <v>0</v>
+      </c>
+      <c r="D3903">
+        <v>0</v>
+      </c>
+      <c r="E3903">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3904" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3904" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3904">
+        <v>25</v>
+      </c>
+      <c r="C3904">
+        <v>1</v>
+      </c>
+      <c r="D3904">
+        <v>1</v>
+      </c>
+      <c r="E3904">
+        <v>5</v>
+      </c>
+      <c r="F3904">
+        <v>900</v>
+      </c>
+      <c r="H3904" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="3905" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3905" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3905">
+        <v>26</v>
+      </c>
+      <c r="C3905">
+        <v>0</v>
+      </c>
+      <c r="D3905">
+        <v>0</v>
+      </c>
+      <c r="E3905">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3906" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3906" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3906">
+        <v>26</v>
+      </c>
+      <c r="C3906">
+        <v>1</v>
+      </c>
+      <c r="D3906">
+        <v>1</v>
+      </c>
+      <c r="E3906">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3907" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3907" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3907">
+        <v>27</v>
+      </c>
+      <c r="C3907">
+        <v>0</v>
+      </c>
+      <c r="D3907">
+        <v>0</v>
+      </c>
+      <c r="E3907">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3908" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3908" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3908">
+        <v>27</v>
+      </c>
+      <c r="C3908">
+        <v>1</v>
+      </c>
+      <c r="D3908">
+        <v>1</v>
+      </c>
+      <c r="E3908">
+        <v>3</v>
+      </c>
+      <c r="F3908">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="3909" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3909" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3909">
+        <v>28</v>
+      </c>
+      <c r="C3909">
+        <v>0</v>
+      </c>
+      <c r="D3909">
+        <v>0</v>
+      </c>
+      <c r="E3909">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3910" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3910" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3910">
+        <v>28</v>
+      </c>
+      <c r="C3910">
+        <v>1</v>
+      </c>
+      <c r="D3910">
+        <v>1</v>
+      </c>
+      <c r="E3910">
+        <v>2</v>
+      </c>
+      <c r="F3910">
+        <v>1800</v>
+      </c>
+      <c r="G3910">
+        <v>8100</v>
+      </c>
+      <c r="H3910" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="3911" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3911" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3911">
+        <v>29</v>
+      </c>
+      <c r="C3911">
+        <v>0</v>
+      </c>
+      <c r="D3911">
+        <v>0</v>
+      </c>
+      <c r="E3911">
+        <v>0</v>
+      </c>
+      <c r="H3911" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3912" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3912" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3912">
+        <v>30</v>
+      </c>
+      <c r="C3912">
+        <v>0</v>
+      </c>
+      <c r="D3912">
+        <v>0</v>
+      </c>
+      <c r="E3912">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3913" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3913" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3913">
+        <v>30</v>
+      </c>
+      <c r="C3913">
+        <v>1</v>
+      </c>
+      <c r="D3913">
+        <v>0</v>
+      </c>
+      <c r="E3913">
+        <v>5</v>
+      </c>
+      <c r="F3913">
+        <v>4500</v>
+      </c>
+      <c r="G3913">
+        <v>13500</v>
+      </c>
+      <c r="H3913" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="3914" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3914" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3914">
+        <v>31</v>
+      </c>
+      <c r="C3914">
+        <v>0</v>
+      </c>
+      <c r="D3914">
+        <v>0</v>
+      </c>
+      <c r="E3914">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3915" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3915" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3915">
+        <v>31</v>
+      </c>
+      <c r="C3915">
+        <v>1</v>
+      </c>
+      <c r="D3915">
+        <v>0</v>
+      </c>
+      <c r="E3915">
+        <v>5</v>
+      </c>
+      <c r="H3915" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="3916" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3916" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3916">
+        <v>32</v>
+      </c>
+      <c r="C3916">
+        <v>0</v>
+      </c>
+      <c r="D3916">
+        <v>0</v>
+      </c>
+      <c r="E3916">
+        <v>0</v>
+      </c>
+      <c r="H3916" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3917" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3917" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3917">
+        <v>33</v>
+      </c>
+      <c r="C3917">
+        <v>0</v>
+      </c>
+      <c r="D3917">
+        <v>0</v>
+      </c>
+      <c r="E3917">
+        <v>0</v>
+      </c>
+      <c r="H3917" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3918" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3918" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3918">
+        <v>34</v>
+      </c>
+      <c r="C3918">
+        <v>0</v>
+      </c>
+      <c r="D3918">
+        <v>0</v>
+      </c>
+      <c r="E3918">
+        <v>0</v>
+      </c>
+      <c r="H3918" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3919" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3919" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3919">
+        <v>35</v>
+      </c>
+      <c r="C3919">
+        <v>0</v>
+      </c>
+      <c r="D3919">
+        <v>0</v>
+      </c>
+      <c r="E3919">
+        <v>0</v>
+      </c>
+      <c r="H3919" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3920" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3920" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3920">
+        <v>36</v>
+      </c>
+      <c r="C3920">
+        <v>0</v>
+      </c>
+      <c r="D3920">
+        <v>0</v>
+      </c>
+      <c r="E3920">
+        <v>0</v>
+      </c>
+      <c r="H3920" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3921" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3921" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3921">
+        <v>37</v>
+      </c>
+      <c r="C3921">
+        <v>0</v>
+      </c>
+      <c r="D3921">
+        <v>0</v>
+      </c>
+      <c r="E3921">
+        <v>0</v>
+      </c>
+      <c r="H3921" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3922" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3922" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3922">
+        <v>37</v>
+      </c>
+      <c r="C3922">
+        <v>1</v>
+      </c>
+      <c r="D3922">
+        <v>0</v>
+      </c>
+      <c r="E3922">
+        <v>3</v>
+      </c>
+      <c r="F3922">
+        <v>900</v>
+      </c>
+      <c r="H3922" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="3923" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3923" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3923">
+        <v>38</v>
+      </c>
+      <c r="C3923">
+        <v>0</v>
+      </c>
+      <c r="D3923">
+        <v>0</v>
+      </c>
+      <c r="E3923">
+        <v>0</v>
+      </c>
+      <c r="H3923" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3924" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3924" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3924">
+        <v>39</v>
+      </c>
+      <c r="C3924">
+        <v>0</v>
+      </c>
+      <c r="D3924">
+        <v>0</v>
+      </c>
+      <c r="E3924">
+        <v>0</v>
+      </c>
+      <c r="H3924" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3925" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3925" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3925">
+        <v>40</v>
+      </c>
+      <c r="C3925">
+        <v>0</v>
+      </c>
+      <c r="D3925">
+        <v>0</v>
+      </c>
+      <c r="E3925">
+        <v>0</v>
+      </c>
+      <c r="H3925" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3926" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3926" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3926">
+        <v>41</v>
+      </c>
+      <c r="C3926">
+        <v>0</v>
+      </c>
+      <c r="D3926">
+        <v>0</v>
+      </c>
+      <c r="E3926">
+        <v>0</v>
+      </c>
+      <c r="H3926" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3927" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3927" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3927">
+        <v>42</v>
+      </c>
+      <c r="C3927">
+        <v>0</v>
+      </c>
+      <c r="D3927">
+        <v>0</v>
+      </c>
+      <c r="E3927">
+        <v>0</v>
+      </c>
+      <c r="H3927" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3928" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3928" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3928">
+        <v>43</v>
+      </c>
+      <c r="C3928">
+        <v>0</v>
+      </c>
+      <c r="D3928">
+        <v>0</v>
+      </c>
+      <c r="E3928">
+        <v>0</v>
+      </c>
+      <c r="H3928" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3929" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3929" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3929">
+        <v>44</v>
+      </c>
+      <c r="C3929">
+        <v>0</v>
+      </c>
+      <c r="D3929">
+        <v>0</v>
+      </c>
+      <c r="E3929">
+        <v>0</v>
+      </c>
+      <c r="H3929" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3930" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3930" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3930">
+        <v>45</v>
+      </c>
+      <c r="C3930">
+        <v>0</v>
+      </c>
+      <c r="D3930">
+        <v>0</v>
+      </c>
+      <c r="E3930">
+        <v>0</v>
+      </c>
+      <c r="H3930" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3931" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3931" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3931">
+        <v>46</v>
+      </c>
+      <c r="C3931">
+        <v>0</v>
+      </c>
+      <c r="D3931">
+        <v>0</v>
+      </c>
+      <c r="E3931">
+        <v>0</v>
+      </c>
+      <c r="H3931" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3932" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3932" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3932">
+        <v>47</v>
+      </c>
+      <c r="C3932">
+        <v>0</v>
+      </c>
+      <c r="D3932">
+        <v>0</v>
+      </c>
+      <c r="E3932">
+        <v>0</v>
+      </c>
+      <c r="H3932" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3933" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3933" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3933">
+        <v>47</v>
+      </c>
+      <c r="C3933">
+        <v>1</v>
+      </c>
+      <c r="D3933">
+        <v>1</v>
+      </c>
+      <c r="E3933">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3934" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3934" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3934">
+        <v>48</v>
+      </c>
+      <c r="C3934">
+        <v>0</v>
+      </c>
+      <c r="D3934">
+        <v>0</v>
+      </c>
+      <c r="E3934">
+        <v>0</v>
+      </c>
+      <c r="H3934" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3935" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3935" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3935">
+        <v>49</v>
+      </c>
+      <c r="C3935">
+        <v>0</v>
+      </c>
+      <c r="D3935">
+        <v>0</v>
+      </c>
+      <c r="E3935">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3936" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3936" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3936">
+        <v>49</v>
+      </c>
+      <c r="C3936">
+        <v>1</v>
+      </c>
+      <c r="D3936">
+        <v>1</v>
+      </c>
+      <c r="E3936">
+        <v>3</v>
+      </c>
+      <c r="F3936">
+        <v>2700</v>
+      </c>
+      <c r="H3936" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="3937" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3937" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3937">
+        <v>50</v>
+      </c>
+      <c r="C3937">
+        <v>0</v>
+      </c>
+      <c r="D3937">
+        <v>0</v>
+      </c>
+      <c r="E3937">
+        <v>0</v>
+      </c>
+      <c r="H3937" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3938" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3938" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3938">
+        <v>51</v>
+      </c>
+      <c r="C3938">
+        <v>0</v>
+      </c>
+      <c r="D3938">
+        <v>0</v>
+      </c>
+      <c r="E3938">
+        <v>0</v>
+      </c>
+      <c r="H3938" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3939" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3939" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3939">
+        <v>52</v>
+      </c>
+      <c r="C3939">
+        <v>0</v>
+      </c>
+      <c r="D3939">
+        <v>0</v>
+      </c>
+      <c r="E3939">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3940" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3940" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3940">
+        <v>53</v>
+      </c>
+      <c r="C3940">
+        <v>0</v>
+      </c>
+      <c r="D3940">
+        <v>0</v>
+      </c>
+      <c r="E3940">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3941" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3941" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3941">
+        <v>53</v>
+      </c>
+      <c r="C3941">
+        <v>1</v>
+      </c>
+      <c r="D3941">
+        <v>0</v>
+      </c>
+      <c r="E3941">
+        <v>2</v>
+      </c>
+      <c r="F3941">
+        <v>7200</v>
+      </c>
+      <c r="H3941" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="3942" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3942" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3942">
+        <v>54</v>
+      </c>
+      <c r="C3942">
+        <v>0</v>
+      </c>
+      <c r="D3942">
+        <v>0</v>
+      </c>
+      <c r="E3942">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3943" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3943" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3943">
+        <v>54</v>
+      </c>
+      <c r="C3943">
+        <v>1</v>
+      </c>
+      <c r="D3943">
+        <v>1</v>
+      </c>
+      <c r="E3943">
+        <v>4</v>
+      </c>
+      <c r="F3943">
+        <v>11700</v>
+      </c>
+      <c r="H3943" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="3944" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3944" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3944">
+        <v>55</v>
+      </c>
+      <c r="C3944">
+        <v>0</v>
+      </c>
+      <c r="D3944">
+        <v>0</v>
+      </c>
+      <c r="E3944">
+        <v>0</v>
+      </c>
+      <c r="H3944" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3945" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3945" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3945">
+        <v>56</v>
+      </c>
+      <c r="C3945">
+        <v>0</v>
+      </c>
+      <c r="D3945">
+        <v>0</v>
+      </c>
+      <c r="E3945">
+        <v>0</v>
+      </c>
+      <c r="H3945" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3946" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3946" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3946">
+        <v>57</v>
+      </c>
+      <c r="C3946">
+        <v>0</v>
+      </c>
+      <c r="D3946">
+        <v>0</v>
+      </c>
+      <c r="E3946">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3947" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3947" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3947">
+        <v>57</v>
+      </c>
+      <c r="C3947">
+        <v>1</v>
+      </c>
+      <c r="D3947">
+        <v>1</v>
+      </c>
+      <c r="E3947">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3948" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3948" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3948">
+        <v>58</v>
+      </c>
+      <c r="C3948">
+        <v>0</v>
+      </c>
+      <c r="D3948">
+        <v>0</v>
+      </c>
+      <c r="E3948">
+        <v>0</v>
+      </c>
+      <c r="H3948" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3949" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3949" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3949">
+        <v>59</v>
+      </c>
+      <c r="C3949">
+        <v>0</v>
+      </c>
+      <c r="D3949">
+        <v>0</v>
+      </c>
+      <c r="E3949">
+        <v>0</v>
+      </c>
+      <c r="H3949" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3950" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3950" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3950">
+        <v>60</v>
+      </c>
+      <c r="C3950">
+        <v>0</v>
+      </c>
+      <c r="D3950">
+        <v>0</v>
+      </c>
+      <c r="E3950">
+        <v>0</v>
+      </c>
+      <c r="H3950" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3951" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3951" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3951">
+        <v>61</v>
+      </c>
+      <c r="C3951">
+        <v>0</v>
+      </c>
+      <c r="D3951">
+        <v>0</v>
+      </c>
+      <c r="E3951">
+        <v>0</v>
+      </c>
+      <c r="H3951" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3952" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3952" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3952">
+        <v>62</v>
+      </c>
+      <c r="C3952">
+        <v>0</v>
+      </c>
+      <c r="D3952">
+        <v>0</v>
+      </c>
+      <c r="E3952">
+        <v>0</v>
+      </c>
+      <c r="H3952" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3953" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3953" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3953">
+        <v>63</v>
+      </c>
+      <c r="C3953">
+        <v>0</v>
+      </c>
+      <c r="D3953">
+        <v>0</v>
+      </c>
+      <c r="E3953">
+        <v>0</v>
+      </c>
+      <c r="H3953" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3954" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3954" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3954">
+        <v>64</v>
+      </c>
+      <c r="C3954">
+        <v>0</v>
+      </c>
+      <c r="D3954">
+        <v>0</v>
+      </c>
+      <c r="E3954">
+        <v>0</v>
+      </c>
+      <c r="H3954" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3955" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3955" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3955">
+        <v>64</v>
+      </c>
+      <c r="C3955">
+        <v>1</v>
+      </c>
+      <c r="D3955">
+        <v>1</v>
+      </c>
+      <c r="E3955">
+        <v>3</v>
+      </c>
+      <c r="F3955">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="3956" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3956" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3956">
+        <v>1</v>
+      </c>
+      <c r="C3956">
+        <v>0</v>
+      </c>
+      <c r="D3956">
+        <v>0</v>
+      </c>
+      <c r="E3956">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3957" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3957" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3957">
+        <v>1</v>
+      </c>
+      <c r="C3957">
+        <v>1</v>
+      </c>
+      <c r="D3957">
+        <v>0</v>
+      </c>
+      <c r="E3957">
+        <v>2</v>
+      </c>
+      <c r="F3957">
+        <v>12600</v>
+      </c>
+      <c r="H3957" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="3958" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3958" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3958">
+        <v>2</v>
+      </c>
+      <c r="C3958">
+        <v>0</v>
+      </c>
+      <c r="D3958">
+        <v>0</v>
+      </c>
+      <c r="E3958">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3959" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3959" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3959">
+        <v>2</v>
+      </c>
+      <c r="C3959">
+        <v>1</v>
+      </c>
+      <c r="D3959">
+        <v>0</v>
+      </c>
+      <c r="E3959">
+        <v>4</v>
+      </c>
+      <c r="F3959">
+        <v>1800</v>
+      </c>
+      <c r="H3959" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="3960" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3960" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3960">
+        <v>3</v>
+      </c>
+      <c r="C3960">
+        <v>0</v>
+      </c>
+      <c r="D3960">
+        <v>0</v>
+      </c>
+      <c r="E3960">
+        <v>0</v>
+      </c>
+      <c r="H3960" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3961" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3961" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3961">
+        <v>4</v>
+      </c>
+      <c r="C3961">
+        <v>0</v>
+      </c>
+      <c r="D3961">
+        <v>0</v>
+      </c>
+      <c r="E3961">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3962" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3962" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3962">
+        <v>4</v>
+      </c>
+      <c r="C3962">
+        <v>1</v>
+      </c>
+      <c r="D3962">
+        <v>1</v>
+      </c>
+      <c r="E3962">
+        <v>3</v>
+      </c>
+      <c r="F3962">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="3963" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3963" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3963">
+        <v>5</v>
+      </c>
+      <c r="C3963">
+        <v>0</v>
+      </c>
+      <c r="D3963">
+        <v>0</v>
+      </c>
+      <c r="E3963">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3964" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3964" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3964">
+        <v>5</v>
+      </c>
+      <c r="C3964">
+        <v>1</v>
+      </c>
+      <c r="D3964">
+        <v>1</v>
+      </c>
+      <c r="E3964">
+        <v>2</v>
+      </c>
+      <c r="F3964">
+        <v>900</v>
+      </c>
+      <c r="G3964">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="3965" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3965" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3965">
+        <v>6</v>
+      </c>
+      <c r="C3965">
+        <v>0</v>
+      </c>
+      <c r="D3965">
+        <v>0</v>
+      </c>
+      <c r="E3965">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3966" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3966" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3966">
+        <v>6</v>
+      </c>
+      <c r="C3966">
+        <v>1</v>
+      </c>
+      <c r="D3966">
+        <v>1</v>
+      </c>
+      <c r="E3966">
+        <v>4</v>
+      </c>
+      <c r="F3966">
+        <v>900</v>
+      </c>
+      <c r="G3966">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="3967" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3967" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3967">
+        <v>7</v>
+      </c>
+      <c r="C3967">
+        <v>0</v>
+      </c>
+      <c r="D3967">
+        <v>0</v>
+      </c>
+      <c r="E3967">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3968" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3968" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3968">
+        <v>7</v>
+      </c>
+      <c r="C3968">
+        <v>1</v>
+      </c>
+      <c r="D3968">
+        <v>1</v>
+      </c>
+      <c r="E3968">
+        <v>4</v>
+      </c>
+      <c r="F3968">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="3969" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3969" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3969">
+        <v>8</v>
+      </c>
+      <c r="C3969">
+        <v>0</v>
+      </c>
+      <c r="D3969">
+        <v>0</v>
+      </c>
+      <c r="E3969">
+        <v>0</v>
+      </c>
+      <c r="H3969" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3970" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3970" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3970">
+        <v>9</v>
+      </c>
+      <c r="C3970">
+        <v>0</v>
+      </c>
+      <c r="D3970">
+        <v>0</v>
+      </c>
+      <c r="E3970">
+        <v>0</v>
+      </c>
+      <c r="H3970" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3971" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3971" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3971">
+        <v>10</v>
+      </c>
+      <c r="C3971">
+        <v>0</v>
+      </c>
+      <c r="D3971">
+        <v>0</v>
+      </c>
+      <c r="E3971">
+        <v>0</v>
+      </c>
+      <c r="H3971" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3972" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3972" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3972">
+        <v>11</v>
+      </c>
+      <c r="C3972">
+        <v>0</v>
+      </c>
+      <c r="D3972">
+        <v>0</v>
+      </c>
+      <c r="E3972">
+        <v>0</v>
+      </c>
+      <c r="H3972" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3973" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3973" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3973">
+        <v>12</v>
+      </c>
+      <c r="C3973">
+        <v>0</v>
+      </c>
+      <c r="D3973">
+        <v>0</v>
+      </c>
+      <c r="E3973">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3974" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3974" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3974">
+        <v>12</v>
+      </c>
+      <c r="C3974">
+        <v>1</v>
+      </c>
+      <c r="D3974">
+        <v>1</v>
+      </c>
+      <c r="E3974">
+        <v>4</v>
+      </c>
+      <c r="F3974">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="3975" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3975" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3975">
+        <v>13</v>
+      </c>
+      <c r="C3975">
+        <v>0</v>
+      </c>
+      <c r="D3975">
+        <v>0</v>
+      </c>
+      <c r="E3975">
+        <v>0</v>
+      </c>
+      <c r="H3975" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3976" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3976" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3976">
+        <v>14</v>
+      </c>
+      <c r="C3976">
+        <v>0</v>
+      </c>
+      <c r="D3976">
+        <v>0</v>
+      </c>
+      <c r="E3976">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3977" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3977" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3977">
+        <v>14</v>
+      </c>
+      <c r="C3977">
+        <v>1</v>
+      </c>
+      <c r="D3977">
+        <v>1</v>
+      </c>
+      <c r="E3977">
+        <v>3</v>
+      </c>
+      <c r="G3977">
+        <v>5400</v>
+      </c>
+      <c r="H3977" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3978" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3978" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3978">
+        <v>15</v>
+      </c>
+      <c r="C3978">
+        <v>0</v>
+      </c>
+      <c r="D3978">
+        <v>0</v>
+      </c>
+      <c r="E3978">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3979" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3979" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3979">
+        <v>15</v>
+      </c>
+      <c r="C3979">
+        <v>1</v>
+      </c>
+      <c r="D3979">
+        <v>1</v>
+      </c>
+      <c r="E3979">
+        <v>3</v>
+      </c>
+      <c r="G3979">
+        <v>8100</v>
+      </c>
+    </row>
+    <row r="3980" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3980" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3980">
+        <v>16</v>
+      </c>
+      <c r="C3980">
+        <v>0</v>
+      </c>
+      <c r="D3980">
+        <v>0</v>
+      </c>
+      <c r="E3980">
+        <v>0</v>
+      </c>
+      <c r="H3980" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3981" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3981" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3981">
+        <v>17</v>
+      </c>
+      <c r="C3981">
+        <v>0</v>
+      </c>
+      <c r="D3981">
+        <v>0</v>
+      </c>
+      <c r="E3981">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3982" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3982" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3982">
+        <v>17</v>
+      </c>
+      <c r="C3982">
+        <v>1</v>
+      </c>
+      <c r="D3982">
+        <v>1</v>
+      </c>
+      <c r="E3982">
+        <v>3</v>
+      </c>
+      <c r="F3982">
+        <v>900</v>
+      </c>
+      <c r="G3982">
+        <v>5400</v>
+      </c>
+      <c r="H3982" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="3983" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3983" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3983">
+        <v>18</v>
+      </c>
+      <c r="C3983">
+        <v>0</v>
+      </c>
+      <c r="D3983">
+        <v>0</v>
+      </c>
+      <c r="E3983">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3984" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3984" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3984">
+        <v>18</v>
+      </c>
+      <c r="C3984">
+        <v>1</v>
+      </c>
+      <c r="D3984">
+        <v>1</v>
+      </c>
+      <c r="E3984">
+        <v>4</v>
+      </c>
+      <c r="F3984">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="3985" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3985" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3985">
+        <v>19</v>
+      </c>
+      <c r="C3985">
+        <v>0</v>
+      </c>
+      <c r="D3985">
+        <v>0</v>
+      </c>
+      <c r="E3985">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3986" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3986" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3986">
+        <v>19</v>
+      </c>
+      <c r="C3986">
+        <v>1</v>
+      </c>
+      <c r="D3986">
+        <v>1</v>
+      </c>
+      <c r="E3986">
+        <v>2</v>
+      </c>
+      <c r="F3986">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="3987" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3987" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3987">
+        <v>20</v>
+      </c>
+      <c r="C3987">
+        <v>0</v>
+      </c>
+      <c r="D3987">
+        <v>0</v>
+      </c>
+      <c r="E3987">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3988" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3988" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3988">
+        <v>20</v>
+      </c>
+      <c r="C3988">
+        <v>1</v>
+      </c>
+      <c r="D3988">
+        <v>1</v>
+      </c>
+      <c r="E3988">
+        <v>3</v>
+      </c>
+      <c r="F3988">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="3989" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3989" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3989">
+        <v>20</v>
+      </c>
+      <c r="C3989">
+        <v>2</v>
+      </c>
+      <c r="D3989">
+        <v>1</v>
+      </c>
+      <c r="E3989">
+        <v>3</v>
+      </c>
+      <c r="F3989">
+        <v>9000</v>
+      </c>
+      <c r="G3989">
+        <v>14400</v>
+      </c>
+      <c r="H3989" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="3990" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3990" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3990">
+        <v>21</v>
+      </c>
+      <c r="C3990">
+        <v>0</v>
+      </c>
+      <c r="D3990">
+        <v>0</v>
+      </c>
+      <c r="E3990">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3991" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3991" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3991">
+        <v>21</v>
+      </c>
+      <c r="C3991">
+        <v>1</v>
+      </c>
+      <c r="D3991">
+        <v>1</v>
+      </c>
+      <c r="E3991">
+        <v>2</v>
+      </c>
+      <c r="F3991">
+        <v>1800</v>
+      </c>
+      <c r="G3991">
+        <v>14400</v>
+      </c>
+    </row>
+    <row r="3992" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3992" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3992">
+        <v>22</v>
+      </c>
+      <c r="C3992">
+        <v>0</v>
+      </c>
+      <c r="D3992">
+        <v>0</v>
+      </c>
+      <c r="E3992">
+        <v>0</v>
+      </c>
+      <c r="H3992" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3993" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3993" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3993">
+        <v>23</v>
+      </c>
+      <c r="C3993">
+        <v>0</v>
+      </c>
+      <c r="D3993">
+        <v>0</v>
+      </c>
+      <c r="E3993">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3994" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3994" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3994">
+        <v>23</v>
+      </c>
+      <c r="C3994">
+        <v>1</v>
+      </c>
+      <c r="D3994">
+        <v>1</v>
+      </c>
+      <c r="E3994">
+        <v>2</v>
+      </c>
+      <c r="F3994">
+        <v>11700</v>
+      </c>
+      <c r="H3994" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="3995" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3995" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3995">
+        <v>24</v>
+      </c>
+      <c r="C3995">
+        <v>0</v>
+      </c>
+      <c r="D3995">
+        <v>0</v>
+      </c>
+      <c r="E3995">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3996" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3996" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3996">
+        <v>24</v>
+      </c>
+      <c r="C3996">
+        <v>1</v>
+      </c>
+      <c r="D3996">
+        <v>1</v>
+      </c>
+      <c r="E3996">
+        <v>4</v>
+      </c>
+      <c r="F3996">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="3997" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3997" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3997">
+        <v>24</v>
+      </c>
+      <c r="C3997">
+        <v>2</v>
+      </c>
+      <c r="D3997">
+        <v>1</v>
+      </c>
+      <c r="E3997">
+        <v>2</v>
+      </c>
+      <c r="F3997">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="3998" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3998" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3998">
+        <v>25</v>
+      </c>
+      <c r="C3998">
+        <v>0</v>
+      </c>
+      <c r="D3998">
+        <v>0</v>
+      </c>
+      <c r="E3998">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3999" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3999" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3999">
+        <v>25</v>
+      </c>
+      <c r="C3999">
+        <v>1</v>
+      </c>
+      <c r="D3999">
+        <v>0</v>
+      </c>
+      <c r="E3999">
+        <v>3</v>
+      </c>
+      <c r="F3999">
+        <v>1800</v>
+      </c>
+      <c r="G3999">
+        <v>9000</v>
+      </c>
+      <c r="H3999" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="4000" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4000" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4000">
+        <v>26</v>
+      </c>
+      <c r="C4000">
+        <v>0</v>
+      </c>
+      <c r="D4000">
+        <v>0</v>
+      </c>
+      <c r="E4000">
+        <v>0</v>
+      </c>
+      <c r="H4000" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="4001" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4001" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4001">
+        <v>27</v>
+      </c>
+      <c r="C4001">
+        <v>0</v>
+      </c>
+      <c r="D4001">
+        <v>0</v>
+      </c>
+      <c r="E4001">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4002" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4002" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4002">
+        <v>27</v>
+      </c>
+      <c r="C4002">
+        <v>1</v>
+      </c>
+      <c r="D4002">
+        <v>0</v>
+      </c>
+      <c r="E4002">
+        <v>3</v>
+      </c>
+      <c r="F4002">
+        <v>6300</v>
+      </c>
+      <c r="H4002" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="4003" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4003" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4003">
+        <v>27</v>
+      </c>
+      <c r="C4003">
+        <v>2</v>
+      </c>
+      <c r="D4003">
+        <v>0</v>
+      </c>
+      <c r="E4003">
+        <v>4</v>
+      </c>
+      <c r="F4003">
+        <v>2700</v>
+      </c>
+      <c r="G4003">
+        <v>4500</v>
+      </c>
+      <c r="H4003" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="4004" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4004" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4004">
+        <v>27</v>
+      </c>
+      <c r="C4004">
+        <v>3</v>
+      </c>
+      <c r="D4004">
+        <v>0</v>
+      </c>
+      <c r="E4004">
+        <v>3</v>
+      </c>
+      <c r="F4004">
+        <v>1800</v>
+      </c>
+      <c r="G4004">
+        <v>2700</v>
+      </c>
+      <c r="H4004" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="4005" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4005" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4005">
+        <v>28</v>
+      </c>
+      <c r="C4005">
+        <v>0</v>
+      </c>
+      <c r="D4005">
+        <v>0</v>
+      </c>
+      <c r="E4005">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4006" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4006" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4006">
+        <v>28</v>
+      </c>
+      <c r="C4006">
+        <v>1</v>
+      </c>
+      <c r="D4006">
+        <v>0</v>
+      </c>
+      <c r="E4006">
+        <v>3</v>
+      </c>
+      <c r="F4006">
+        <v>900</v>
+      </c>
+      <c r="G4006">
+        <v>6300</v>
+      </c>
+      <c r="H4006" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="4007" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4007" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4007">
+        <v>29</v>
+      </c>
+      <c r="C4007">
+        <v>0</v>
+      </c>
+      <c r="D4007">
+        <v>0</v>
+      </c>
+      <c r="E4007">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4008" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4008" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4008">
+        <v>29</v>
+      </c>
+      <c r="C4008">
+        <v>1</v>
+      </c>
+      <c r="D4008">
+        <v>0</v>
+      </c>
+      <c r="E4008">
+        <v>5</v>
+      </c>
+      <c r="G4008">
+        <v>8100</v>
+      </c>
+      <c r="H4008" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="4009" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4009" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4009">
+        <v>29</v>
+      </c>
+      <c r="C4009">
+        <v>2</v>
+      </c>
+      <c r="D4009">
+        <v>0</v>
+      </c>
+      <c r="E4009">
+        <v>5</v>
+      </c>
+      <c r="G4009">
+        <v>3600</v>
+      </c>
+      <c r="H4009" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="4010" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4010" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4010">
+        <v>30</v>
+      </c>
+      <c r="C4010">
+        <v>0</v>
+      </c>
+      <c r="D4010">
+        <v>0</v>
+      </c>
+      <c r="E4010">
+        <v>0</v>
+      </c>
+      <c r="H4010" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4011" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4011" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4011">
+        <v>31</v>
+      </c>
+      <c r="C4011">
+        <v>0</v>
+      </c>
+      <c r="D4011">
+        <v>0</v>
+      </c>
+      <c r="E4011">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4012" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4012" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4012">
+        <v>31</v>
+      </c>
+      <c r="C4012">
+        <v>1</v>
+      </c>
+      <c r="D4012">
+        <v>0</v>
+      </c>
+      <c r="E4012">
+        <v>3</v>
+      </c>
+      <c r="F4012">
+        <v>2700</v>
+      </c>
+      <c r="G4012">
+        <v>7200</v>
+      </c>
+      <c r="H4012" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="4013" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4013" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4013">
+        <v>31</v>
+      </c>
+      <c r="C4013">
+        <v>2</v>
+      </c>
+      <c r="D4013">
+        <v>1</v>
+      </c>
+      <c r="E4013">
+        <v>3</v>
+      </c>
+      <c r="F4013">
+        <v>8100</v>
+      </c>
+    </row>
+    <row r="4014" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4014" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4014">
+        <v>32</v>
+      </c>
+      <c r="C4014">
+        <v>0</v>
+      </c>
+      <c r="D4014">
+        <v>0</v>
+      </c>
+      <c r="E4014">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4015" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4015" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4015">
+        <v>32</v>
+      </c>
+      <c r="C4015">
+        <v>1</v>
+      </c>
+      <c r="D4015">
+        <v>1</v>
+      </c>
+      <c r="E4015">
+        <v>3</v>
+      </c>
+      <c r="H4015" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4016" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4016" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4016">
+        <v>33</v>
+      </c>
+      <c r="C4016">
+        <v>0</v>
+      </c>
+      <c r="D4016">
+        <v>0</v>
+      </c>
+      <c r="E4016">
+        <v>0</v>
+      </c>
+      <c r="H4016" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4017" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4017" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4017">
+        <v>34</v>
+      </c>
+      <c r="C4017">
+        <v>0</v>
+      </c>
+      <c r="D4017">
+        <v>0</v>
+      </c>
+      <c r="E4017">
+        <v>0</v>
+      </c>
+      <c r="H4017" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4018" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4018" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4018">
+        <v>35</v>
+      </c>
+      <c r="C4018">
+        <v>0</v>
+      </c>
+      <c r="D4018">
+        <v>0</v>
+      </c>
+      <c r="E4018">
+        <v>0</v>
+      </c>
+      <c r="H4018" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4019" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4019" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4019">
+        <v>36</v>
+      </c>
+      <c r="C4019">
+        <v>0</v>
+      </c>
+      <c r="D4019">
+        <v>0</v>
+      </c>
+      <c r="E4019">
+        <v>0</v>
+      </c>
+      <c r="H4019" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4020" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4020" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4020">
+        <v>37</v>
+      </c>
+      <c r="C4020">
+        <v>0</v>
+      </c>
+      <c r="D4020">
+        <v>0</v>
+      </c>
+      <c r="E4020">
+        <v>0</v>
+      </c>
+      <c r="H4020" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4021" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4021" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4021">
+        <v>38</v>
+      </c>
+      <c r="C4021">
+        <v>0</v>
+      </c>
+      <c r="D4021">
+        <v>0</v>
+      </c>
+      <c r="E4021">
+        <v>0</v>
+      </c>
+      <c r="H4021" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4022" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4022" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4022">
+        <v>39</v>
+      </c>
+      <c r="C4022">
+        <v>0</v>
+      </c>
+      <c r="D4022">
+        <v>0</v>
+      </c>
+      <c r="E4022">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4023" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4023" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4023">
+        <v>39</v>
+      </c>
+      <c r="C4023">
+        <v>1</v>
+      </c>
+      <c r="D4023">
+        <v>0</v>
+      </c>
+      <c r="E4023">
+        <v>3</v>
+      </c>
+      <c r="F4023">
+        <v>3600</v>
+      </c>
+      <c r="H4023" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="4024" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4024" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4024">
+        <v>40</v>
+      </c>
+      <c r="C4024">
+        <v>0</v>
+      </c>
+      <c r="D4024">
+        <v>0</v>
+      </c>
+      <c r="E4024">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4025" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4025" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4025">
+        <v>40</v>
+      </c>
+      <c r="C4025">
+        <v>1</v>
+      </c>
+      <c r="D4025">
+        <v>1</v>
+      </c>
+      <c r="E4025">
+        <v>3</v>
+      </c>
+      <c r="G4025">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="4026" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4026" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4026">
+        <v>41</v>
+      </c>
+      <c r="C4026">
+        <v>0</v>
+      </c>
+      <c r="D4026">
+        <v>0</v>
+      </c>
+      <c r="E4026">
+        <v>0</v>
+      </c>
+      <c r="H4026" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4027" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4027" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4027">
+        <v>42</v>
+      </c>
+      <c r="C4027">
+        <v>0</v>
+      </c>
+      <c r="D4027">
+        <v>0</v>
+      </c>
+      <c r="E4027">
+        <v>0</v>
+      </c>
+      <c r="H4027" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4028" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4028" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4028">
+        <v>43</v>
+      </c>
+      <c r="C4028">
+        <v>0</v>
+      </c>
+      <c r="D4028">
+        <v>0</v>
+      </c>
+      <c r="E4028">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4029" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4029" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4029">
+        <v>43</v>
+      </c>
+      <c r="C4029">
+        <v>1</v>
+      </c>
+      <c r="D4029">
+        <v>1</v>
+      </c>
+      <c r="E4029">
+        <v>4</v>
+      </c>
+      <c r="G4029">
+        <v>6300</v>
+      </c>
+      <c r="H4029" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="4030" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4030" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4030">
+        <v>43</v>
+      </c>
+      <c r="C4030">
+        <v>2</v>
+      </c>
+      <c r="D4030">
+        <v>1</v>
+      </c>
+      <c r="E4030">
+        <v>5</v>
+      </c>
+      <c r="G4030">
+        <v>2700</v>
+      </c>
+      <c r="H4030" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="4031" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4031" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4031">
+        <v>43</v>
+      </c>
+      <c r="C4031">
+        <v>3</v>
+      </c>
+      <c r="D4031">
+        <v>1</v>
+      </c>
+      <c r="E4031">
+        <v>3</v>
+      </c>
+      <c r="F4031">
+        <v>2700</v>
+      </c>
+      <c r="G4031">
+        <v>5400</v>
+      </c>
+      <c r="H4031" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="4032" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4032" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4032">
+        <v>43</v>
+      </c>
+      <c r="C4032">
+        <v>4</v>
+      </c>
+      <c r="D4032">
+        <v>0</v>
+      </c>
+      <c r="E4032">
+        <v>3</v>
+      </c>
+      <c r="F4032">
+        <v>2700</v>
+      </c>
+      <c r="G4032">
+        <v>5400</v>
+      </c>
+      <c r="H4032" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="4033" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4033" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4033">
+        <v>44</v>
+      </c>
+      <c r="C4033">
+        <v>0</v>
+      </c>
+      <c r="D4033">
+        <v>0</v>
+      </c>
+      <c r="E4033">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4034" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4034" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4034">
+        <v>44</v>
+      </c>
+      <c r="C4034">
+        <v>1</v>
+      </c>
+      <c r="D4034">
+        <v>1</v>
+      </c>
+      <c r="E4034">
+        <v>2</v>
+      </c>
+      <c r="G4034">
+        <v>6300</v>
+      </c>
+      <c r="H4034" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4035" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4035" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4035">
+        <v>45</v>
+      </c>
+      <c r="C4035">
+        <v>0</v>
+      </c>
+      <c r="D4035">
+        <v>0</v>
+      </c>
+      <c r="E4035">
+        <v>0</v>
+      </c>
+      <c r="H4035" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4036" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4036" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4036">
+        <v>46</v>
+      </c>
+      <c r="C4036">
+        <v>0</v>
+      </c>
+      <c r="D4036">
+        <v>0</v>
+      </c>
+      <c r="E4036">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4037" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4037" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4037">
+        <v>46</v>
+      </c>
+      <c r="C4037">
+        <v>1</v>
+      </c>
+      <c r="D4037">
+        <v>1</v>
+      </c>
+      <c r="E4037">
+        <v>2</v>
+      </c>
+      <c r="G4037">
+        <v>14400</v>
+      </c>
+      <c r="H4037" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4038" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4038" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4038">
+        <v>47</v>
+      </c>
+      <c r="C4038">
+        <v>0</v>
+      </c>
+      <c r="D4038">
+        <v>0</v>
+      </c>
+      <c r="E4038">
+        <v>0</v>
+      </c>
+      <c r="H4038" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4039" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4039" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4039">
+        <v>48</v>
+      </c>
+      <c r="C4039">
+        <v>0</v>
+      </c>
+      <c r="D4039">
+        <v>0</v>
+      </c>
+      <c r="E4039">
+        <v>0</v>
+      </c>
+      <c r="H4039" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4040" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4040" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4040">
+        <v>49</v>
+      </c>
+      <c r="C4040">
+        <v>0</v>
+      </c>
+      <c r="D4040">
+        <v>0</v>
+      </c>
+      <c r="E4040">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4041" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4041" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4041">
+        <v>49</v>
+      </c>
+      <c r="C4041">
+        <v>1</v>
+      </c>
+      <c r="D4041">
+        <v>1</v>
+      </c>
+      <c r="E4041">
+        <v>2</v>
+      </c>
+      <c r="F4041">
+        <v>6300</v>
+      </c>
+    </row>
+    <row r="4042" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4042" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4042">
+        <v>50</v>
+      </c>
+      <c r="C4042">
+        <v>0</v>
+      </c>
+      <c r="D4042">
+        <v>0</v>
+      </c>
+      <c r="E4042">
+        <v>0</v>
+      </c>
+      <c r="H4042" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4043" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4043" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4043">
+        <v>51</v>
+      </c>
+      <c r="C4043">
+        <v>0</v>
+      </c>
+      <c r="D4043">
+        <v>0</v>
+      </c>
+      <c r="E4043">
+        <v>0</v>
+      </c>
+      <c r="H4043" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4044" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4044" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4044">
+        <v>52</v>
+      </c>
+      <c r="C4044">
+        <v>0</v>
+      </c>
+      <c r="D4044">
+        <v>0</v>
+      </c>
+      <c r="E4044">
+        <v>0</v>
+      </c>
+      <c r="H4044" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4045" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4045" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4045">
+        <v>53</v>
+      </c>
+      <c r="C4045">
+        <v>0</v>
+      </c>
+      <c r="D4045">
+        <v>0</v>
+      </c>
+      <c r="E4045">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4046" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4046" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4046">
+        <v>53</v>
+      </c>
+      <c r="C4046">
+        <v>1</v>
+      </c>
+      <c r="D4046">
+        <v>1</v>
+      </c>
+      <c r="E4046">
+        <v>3</v>
+      </c>
+      <c r="F4046">
+        <v>8100</v>
+      </c>
+    </row>
+    <row r="4047" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4047" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4047">
+        <v>54</v>
+      </c>
+      <c r="C4047">
+        <v>0</v>
+      </c>
+      <c r="D4047">
+        <v>0</v>
+      </c>
+      <c r="E4047">
+        <v>0</v>
+      </c>
+      <c r="H4047" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4048" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4048" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4048">
+        <v>55</v>
+      </c>
+      <c r="C4048">
+        <v>0</v>
+      </c>
+      <c r="D4048">
+        <v>0</v>
+      </c>
+      <c r="E4048">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4049" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4049" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4049">
+        <v>55</v>
+      </c>
+      <c r="C4049">
+        <v>1</v>
+      </c>
+      <c r="D4049">
+        <v>1</v>
+      </c>
+      <c r="E4049">
+        <v>3</v>
+      </c>
+      <c r="F4049">
+        <v>900</v>
+      </c>
+      <c r="G4049">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="4050" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4050" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4050">
+        <v>55</v>
+      </c>
+      <c r="C4050">
+        <v>2</v>
+      </c>
+      <c r="D4050">
+        <v>0</v>
+      </c>
+      <c r="E4050">
+        <v>4</v>
+      </c>
+      <c r="F4050">
+        <v>1800</v>
+      </c>
+      <c r="G4050">
+        <v>9900</v>
+      </c>
+      <c r="H4050" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="4051" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4051" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4051">
+        <v>55</v>
+      </c>
+      <c r="C4051">
+        <v>3</v>
+      </c>
+      <c r="D4051">
+        <v>0</v>
+      </c>
+      <c r="E4051">
+        <v>3</v>
+      </c>
+      <c r="F4051">
+        <v>1800</v>
+      </c>
+      <c r="G4051">
+        <v>4500</v>
+      </c>
+      <c r="H4051" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="4052" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4052" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4052">
+        <v>55</v>
+      </c>
+      <c r="C4052">
+        <v>4</v>
+      </c>
+      <c r="D4052">
+        <v>0</v>
+      </c>
+      <c r="E4052">
+        <v>2</v>
+      </c>
+      <c r="F4052">
+        <v>1800</v>
+      </c>
+      <c r="G4052">
+        <v>4500</v>
+      </c>
+      <c r="H4052" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="4053" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4053" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4053">
+        <v>55</v>
+      </c>
+      <c r="C4053">
+        <v>5</v>
+      </c>
+      <c r="D4053">
+        <v>0</v>
+      </c>
+      <c r="E4053">
+        <v>4</v>
+      </c>
+      <c r="F4053">
+        <v>5400</v>
+      </c>
+      <c r="G4053">
+        <v>9000</v>
+      </c>
+      <c r="H4053" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="4054" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4054" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4054">
+        <v>56</v>
+      </c>
+      <c r="C4054">
+        <v>0</v>
+      </c>
+      <c r="D4054">
+        <v>0</v>
+      </c>
+      <c r="E4054">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4055" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4055" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4055">
+        <v>56</v>
+      </c>
+      <c r="C4055">
+        <v>1</v>
+      </c>
+      <c r="D4055">
+        <v>1</v>
+      </c>
+      <c r="E4055">
+        <v>3</v>
+      </c>
+      <c r="F4055">
+        <v>1800</v>
+      </c>
+      <c r="G4055">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="4056" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4056" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4056">
+        <v>57</v>
+      </c>
+      <c r="C4056">
+        <v>0</v>
+      </c>
+      <c r="D4056">
+        <v>0</v>
+      </c>
+      <c r="E4056">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4057" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4057" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4057">
+        <v>57</v>
+      </c>
+      <c r="C4057">
+        <v>1</v>
+      </c>
+      <c r="D4057">
+        <v>0</v>
+      </c>
+      <c r="E4057">
+        <v>5</v>
+      </c>
+      <c r="G4057">
+        <v>9000</v>
+      </c>
+      <c r="H4057" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="4058" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4058" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4058">
+        <v>58</v>
+      </c>
+      <c r="C4058">
+        <v>0</v>
+      </c>
+      <c r="D4058">
+        <v>0</v>
+      </c>
+      <c r="E4058">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4059" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4059" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4059">
+        <v>58</v>
+      </c>
+      <c r="C4059">
+        <v>1</v>
+      </c>
+      <c r="D4059">
+        <v>0</v>
+      </c>
+      <c r="E4059">
+        <v>3</v>
+      </c>
+      <c r="F4059">
+        <v>2700</v>
+      </c>
+      <c r="G4059">
+        <v>6300</v>
+      </c>
+      <c r="H4059" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="4060" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4060" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4060">
+        <v>58</v>
+      </c>
+      <c r="C4060">
+        <v>2</v>
+      </c>
+      <c r="D4060">
+        <v>0</v>
+      </c>
+      <c r="E4060">
+        <v>3</v>
+      </c>
+      <c r="F4060">
+        <v>5400</v>
+      </c>
+      <c r="H4060" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="4061" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4061" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4061">
+        <v>59</v>
+      </c>
+      <c r="C4061">
+        <v>0</v>
+      </c>
+      <c r="D4061">
+        <v>0</v>
+      </c>
+      <c r="E4061">
+        <v>0</v>
+      </c>
+      <c r="H4061" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4062" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4062" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4062">
+        <v>60</v>
+      </c>
+      <c r="C4062">
+        <v>0</v>
+      </c>
+      <c r="D4062">
+        <v>0</v>
+      </c>
+      <c r="E4062">
+        <v>0</v>
+      </c>
+      <c r="H4062" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4063" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4063" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4063">
+        <v>61</v>
+      </c>
+      <c r="C4063">
+        <v>0</v>
+      </c>
+      <c r="D4063">
+        <v>0</v>
+      </c>
+      <c r="E4063">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4064" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4064" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4064">
+        <v>61</v>
+      </c>
+      <c r="C4064">
+        <v>1</v>
+      </c>
+      <c r="D4064">
+        <v>1</v>
+      </c>
+      <c r="E4064">
+        <v>3</v>
+      </c>
+      <c r="G4064">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="4065" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4065" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4065">
+        <v>62</v>
+      </c>
+      <c r="C4065">
+        <v>0</v>
+      </c>
+      <c r="D4065">
+        <v>0</v>
+      </c>
+      <c r="E4065">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4066" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4066" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4066">
+        <v>62</v>
+      </c>
+      <c r="C4066">
+        <v>1</v>
+      </c>
+      <c r="D4066">
+        <v>0</v>
+      </c>
+      <c r="E4066">
+        <v>5</v>
+      </c>
+      <c r="F4066">
+        <v>3600</v>
+      </c>
+      <c r="H4066" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="4067" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4067" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4067">
+        <v>62</v>
+      </c>
+      <c r="C4067">
+        <v>2</v>
+      </c>
+      <c r="D4067">
+        <v>1</v>
+      </c>
+      <c r="E4067">
+        <v>2</v>
+      </c>
+      <c r="F4067">
+        <v>5400</v>
+      </c>
+      <c r="G4067">
+        <v>8100</v>
+      </c>
+      <c r="H4067" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4068" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4068" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4068">
+        <v>63</v>
+      </c>
+      <c r="C4068">
+        <v>0</v>
+      </c>
+      <c r="D4068">
+        <v>0</v>
+      </c>
+      <c r="E4068">
+        <v>0</v>
+      </c>
+      <c r="H4068" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4069" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4069" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4069">
+        <v>64</v>
+      </c>
+      <c r="C4069">
+        <v>0</v>
+      </c>
+      <c r="D4069">
+        <v>0</v>
+      </c>
+      <c r="E4069">
+        <v>0</v>
+      </c>
+      <c r="H4069" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make start time and end time cols numeric again
</commit_message>
<xml_diff>
--- a/spikeSortingNotes.xlsx
+++ b/spikeSortingNotes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\MATLAB\gratings-task-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC30241E-CA4A-4EC2-8811-CEA4A6C4DAFA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB729E88-D0BF-4FA9-9786-9E627808CBC3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="645" windowWidth="22485" windowHeight="14955" xr2:uid="{F5215BA6-879C-42E2-A238-7256D4555DD7}"/>
   </bookViews>
@@ -1524,12 +1524,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1847,12 +1849,13 @@
   <dimension ref="A1:H4069"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F1" sqref="F1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="4"/>
     <col min="8" max="8" width="70.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1872,10 +1875,10 @@
       <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>279</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1896,6 +1899,12 @@
         <v>0</v>
       </c>
       <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
         <v>0</v>
       </c>
       <c r="H2" t="s">

</xml_diff>

<commit_message>
fix bad end time
</commit_message>
<xml_diff>
--- a/spikeSortingNotes.xlsx
+++ b/spikeSortingNotes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\MATLAB\gratings-task-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7916FBB-D39F-405D-A9CB-C90EEC247ED2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3358D2-821E-4CDF-8A41-83E286A7DD42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{F5215BA6-879C-42E2-A238-7256D4555DD7}"/>
+    <workbookView xWindow="3780" yWindow="240" windowWidth="24660" windowHeight="14550" xr2:uid="{F5215BA6-879C-42E2-A238-7256D4555DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Unit Info" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,12 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1885,8 +1891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991F1F63-41CC-4425-B140-2A823B1406A8}">
   <dimension ref="A1:H4069"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2810" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A2684" workbookViewId="0">
+      <selection activeCell="F2719" sqref="F2719:G2719"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51800,12 +51806,6 @@
       </c>
       <c r="E2719">
         <v>4</v>
-      </c>
-      <c r="F2719">
-        <v>1800</v>
-      </c>
-      <c r="G2719">
-        <v>2700</v>
       </c>
     </row>
     <row r="2720" spans="1:8" x14ac:dyDescent="0.25">
@@ -78492,7 +78492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C959004D-4D9F-441D-939C-D0A39F61DFAD}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
@@ -78575,7 +78575,7 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:J9" si="0">D3+E3+F3</f>
+        <f t="shared" ref="H3:H9" si="0">D3+E3+F3</f>
         <v>3</v>
       </c>
       <c r="I3">
@@ -78763,7 +78763,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <f t="shared" ref="H8:J8" si="3">D8+E8+F8</f>
+        <f t="shared" ref="H8" si="3">D8+E8+F8</f>
         <v>29</v>
       </c>
       <c r="I8">
@@ -78840,7 +78840,7 @@
         <v>3</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H10:J15" si="4">D10+E10+F10</f>
+        <f t="shared" ref="H10:H15" si="4">D10+E10+F10</f>
         <v>15</v>
       </c>
       <c r="I10">
@@ -79068,7 +79068,7 @@
         <v>8</v>
       </c>
       <c r="H16">
-        <f t="shared" ref="H16:J16" si="5">D16+E16+F16</f>
+        <f t="shared" ref="H16" si="5">D16+E16+F16</f>
         <v>89</v>
       </c>
       <c r="I16">
@@ -79108,7 +79108,7 @@
         <v>7</v>
       </c>
       <c r="H17">
-        <f t="shared" ref="H17:J17" si="6">D17+E17+F17</f>
+        <f t="shared" ref="H17" si="6">D17+E17+F17</f>
         <v>80</v>
       </c>
       <c r="I17">
@@ -79148,7 +79148,7 @@
         <v>1</v>
       </c>
       <c r="H18">
-        <f t="shared" ref="H18:J21" si="7">D18+E18+F18</f>
+        <f t="shared" ref="H18:H21" si="7">D18+E18+F18</f>
         <v>36</v>
       </c>
       <c r="I18">
@@ -79302,7 +79302,7 @@
         <v>0</v>
       </c>
       <c r="H22">
-        <f t="shared" ref="H22:J33" si="8">D22+E22+F22</f>
+        <f t="shared" ref="H22:H33" si="8">D22+E22+F22</f>
         <v>6</v>
       </c>
       <c r="I22">

</xml_diff>

<commit_message>
add color coding to spike sorting sheet
</commit_message>
<xml_diff>
--- a/spikeSortingNotes.xlsx
+++ b/spikeSortingNotes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\MATLAB\gratings-task-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA24F13-7155-443F-A86C-7CE45C9F9E1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398384B6-2A08-44AE-B9D2-733228B1ECBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="240" windowWidth="24660" windowHeight="14550" xr2:uid="{F5215BA6-879C-42E2-A238-7256D4555DD7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5215BA6-879C-42E2-A238-7256D4555DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Unit Info" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1579,7 +1581,146 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1891,8 +2032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991F1F63-41CC-4425-B140-2A823B1406A8}">
   <dimension ref="A1:H4069"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2878" workbookViewId="0">
-      <selection activeCell="F2891" sqref="F2891"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -78471,6 +78612,21 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:A4069" xr:uid="{44851FFE-30DC-4E12-8296-FFBBC3B7B99C}"/>
+  <conditionalFormatting sqref="D2:D1048576">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E1048576">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
+      <formula>2.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND($D1=1,$E1&gt;2)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix start time for F20171017 31a
</commit_message>
<xml_diff>
--- a/spikeSortingNotes.xlsx
+++ b/spikeSortingNotes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\MATLAB\gratings-task-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398384B6-2A08-44AE-B9D2-733228B1ECBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB365F42-7276-4C73-A3C3-D0250EBCBFBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5215BA6-879C-42E2-A238-7256D4555DD7}"/>
   </bookViews>
@@ -1581,122 +1581,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2032,8 +1921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991F1F63-41CC-4425-B140-2A823B1406A8}">
   <dimension ref="A1:H4069"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A3105" workbookViewId="0">
+      <selection activeCell="F3136" sqref="F3136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60054,9 +59943,6 @@
       <c r="E3136">
         <v>4</v>
       </c>
-      <c r="F3136">
-        <v>3600</v>
-      </c>
     </row>
     <row r="3137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3137" t="s">
@@ -78613,12 +78499,12 @@
   </sheetData>
   <autoFilter ref="A1:A4069" xr:uid="{44851FFE-30DC-4E12-8296-FFBBC3B7B99C}"/>
   <conditionalFormatting sqref="D2:D1048576">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E1048576">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
       <formula>2.5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>